<commit_message>
test methode für setUnternehmenData, getUnternhemenData, setRaumData, getRaumData
</commit_message>
<xml_diff>
--- a/src/test/resources/de/bwvaachen/botscheduler/IMPORT BOT0_Raumliste.xlsx
+++ b/src/test/resources/de/bwvaachen/botscheduler/IMPORT BOT0_Raumliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atze\git\BOT-Projekt\BOT-Projekt\src\test\resources\de\bwvaachen\botscheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\+++Schule\AE_LF12\Projekt Berufsorientierungstag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667E12F3-EF98-4944-9D1E-497D0055B887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5638207B-B2F4-4EBA-AE4A-10B5D249FBAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="23040" windowHeight="12168" xr2:uid="{254B5C5A-C805-468E-BF4E-A3CDD66F8374}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" xr2:uid="{254B5C5A-C805-468E-BF4E-A3CDD66F8374}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>008</t>
   </si>
   <si>
     <t>Aula</t>
+  </si>
+  <si>
+    <t>Raum</t>
+  </si>
+  <si>
+    <t>Kapazität</t>
   </si>
 </sst>
 </file>
@@ -87,9 +93,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -127,7 +133,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -233,7 +239,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -375,7 +381,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -383,123 +389,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0EFAA5-628D-4D52-9815-787F64D78A8F}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="B2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>101</v>
       </c>
-      <c r="B2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>102</v>
       </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="B4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>103</v>
       </c>
-      <c r="B4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="B5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>106</v>
       </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="B6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>107</v>
       </c>
-      <c r="B6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="B7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>108</v>
       </c>
-      <c r="B7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="B8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>109</v>
       </c>
-      <c r="B8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="B9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>110</v>
       </c>
-      <c r="B9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="B10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>111</v>
       </c>
-      <c r="B10">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="B11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>112</v>
       </c>
-      <c r="B11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="B12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>113</v>
       </c>
-      <c r="B12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>209</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed roomnumber bug, aggressive swapping,
</commit_message>
<xml_diff>
--- a/src/test/resources/de/bwvaachen/botscheduler/IMPORT BOT0_Raumliste.xlsx
+++ b/src/test/resources/de/bwvaachen/botscheduler/IMPORT BOT0_Raumliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Atze\git\BOT-Projekt\BOT-Projekt\src\test\resources\de\bwvaachen\botscheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\+++Schule\AE_LF12\Projekt Berufsorientierungstag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667E12F3-EF98-4944-9D1E-497D0055B887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5638207B-B2F4-4EBA-AE4A-10B5D249FBAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="23040" windowHeight="12168" xr2:uid="{254B5C5A-C805-468E-BF4E-A3CDD66F8374}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" xr2:uid="{254B5C5A-C805-468E-BF4E-A3CDD66F8374}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>008</t>
   </si>
   <si>
     <t>Aula</t>
+  </si>
+  <si>
+    <t>Raum</t>
+  </si>
+  <si>
+    <t>Kapazität</t>
   </si>
 </sst>
 </file>
@@ -87,9 +93,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -127,7 +133,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -233,7 +239,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -375,7 +381,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -383,123 +389,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0EFAA5-628D-4D52-9815-787F64D78A8F}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="B2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>101</v>
       </c>
-      <c r="B2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>102</v>
       </c>
-      <c r="B3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="B4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>103</v>
       </c>
-      <c r="B4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="B5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>106</v>
       </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="B6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>107</v>
       </c>
-      <c r="B6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="B7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>108</v>
       </c>
-      <c r="B7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="B8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>109</v>
       </c>
-      <c r="B8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="B9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>110</v>
       </c>
-      <c r="B9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="B10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>111</v>
       </c>
-      <c r="B10">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="B11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>112</v>
       </c>
-      <c r="B11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="B12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>113</v>
       </c>
-      <c r="B12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>209</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>20</v>
       </c>
     </row>

</xml_diff>